<commit_message>
Updated final report with graph and changes
</commit_message>
<xml_diff>
--- a/FinalModel/Eval Sheets/ax4_200epochs_learningrate0.01.xlsx
+++ b/FinalModel/Eval Sheets/ax4_200epochs_learningrate0.01.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="predicted_rankings" sheetId="1" r:id="rId1"/>
     <sheet name="evaluation" sheetId="2" r:id="rId2"/>
+    <sheet name="validation graph" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="1244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="1247">
   <si>
     <t>song_title</t>
   </si>
@@ -3757,6 +3758,15 @@
   </si>
   <si>
     <t>1, 10, 13, 21, 41</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Winners</t>
+  </si>
+  <si>
+    <t>Nominees</t>
   </si>
 </sst>
 </file>
@@ -3811,6 +3821,1142 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Predicted Rankings from Validation:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2011-2015</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nominees</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'validation graph'!$A$9:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'validation graph'!$B$9:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Winners</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'validation graph'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'validation graph'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="797334704"/>
+        <c:axId val="797336880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="797334704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2015"/>
+          <c:min val="2011"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797336880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="797336880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797334704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3174</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45043,8 +46189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45242,4 +46388,258 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2011</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2012</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2011</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2011</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2011</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2011</v>
+      </c>
+      <c r="B12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2012</v>
+      </c>
+      <c r="B17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2012</v>
+      </c>
+      <c r="B18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2013</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2014</v>
+      </c>
+      <c r="B24">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2015</v>
+      </c>
+      <c r="B29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2015</v>
+      </c>
+      <c r="B30">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>